<commit_message>
editing old code to fit task 1 (in progress)
</commit_message>
<xml_diff>
--- a/Assignment 1/data/gen_costs.xlsx
+++ b/Assignment 1/data/gen_costs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Dropbox\DTU\46750 - Optimization in Modern Power Systems\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Documents\GitHub\46750\Assignment 2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB671EC-64B1-4AED-804F-94DD0935193D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E86D60D-9E50-4401-A2E1-9EE15CA9D9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{85C15B4B-82FA-45B8-AC78-DFFA9F057C5D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Unit #</t>
   </si>
@@ -144,99 +144,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>($/MWh)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>su ($)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">P </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ini </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(MW)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">U </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ini </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(0/1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">T </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ini </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(h)</t>
     </r>
   </si>
 </sst>
@@ -313,19 +220,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -336,17 +237,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -665,16 +560,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8C6147-0497-45D0-8C63-082C2A1F4918}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -692,401 +587,245 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>13.32</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="4">
         <v>15</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>15</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>11</v>
       </c>
-      <c r="G2" s="1">
-        <v>1430.4</v>
-      </c>
-      <c r="H2" s="8">
-        <v>76</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>13.32</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>15</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>15</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>11</v>
       </c>
-      <c r="G3" s="1">
-        <v>1430.4</v>
-      </c>
-      <c r="H3" s="8">
-        <v>76</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>20.7</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>24</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>16</v>
       </c>
-      <c r="G4" s="1">
-        <v>1725</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>20.93</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>8</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>7</v>
       </c>
       <c r="E5" s="1">
         <v>25</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>17</v>
       </c>
-      <c r="G5" s="1">
-        <v>3056.7</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>26.11</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>7</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>5</v>
       </c>
       <c r="E6" s="1">
         <v>28</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>23</v>
       </c>
-      <c r="G6" s="1">
-        <v>437</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>10.52</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>16</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>16</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <v>7</v>
       </c>
-      <c r="G7" s="1">
-        <v>312</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>10.52</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>16</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>14</v>
       </c>
       <c r="E8" s="1">
         <v>16</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>7</v>
       </c>
-      <c r="G8" s="1">
-        <v>312</v>
-      </c>
-      <c r="H8" s="8">
-        <v>124</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>6.02</v>
       </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
         <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="8">
-        <v>240</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>5.47</v>
       </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
         <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8">
-        <v>240</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
         <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="7">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <v>240</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>10.52</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>17</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>16</v>
       </c>
       <c r="E12" s="1">
         <v>14</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <v>8</v>
       </c>
-      <c r="G12" s="1">
-        <v>624</v>
-      </c>
-      <c r="H12" s="8">
-        <v>248</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>10.89</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="6">
         <v>16</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>14</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>16</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>8</v>
-      </c>
-      <c r="G13" s="5">
-        <v>2298</v>
-      </c>
-      <c r="H13" s="11">
-        <v>280</v>
-      </c>
-      <c r="I13" s="5">
-        <v>1</v>
-      </c>
-      <c r="J13" s="10">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>